<commit_message>
made some changes in each files
</commit_message>
<xml_diff>
--- a/student_platunov/hello_platunov.xlsx
+++ b/student_platunov/hello_platunov.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A39D91-2032-494C-8A47-42000B734B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,14 +19,30 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>First change</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -49,8 +66,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +350,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes after git tag
</commit_message>
<xml_diff>
--- a/student_platunov/hello_platunov.xlsx
+++ b/student_platunov/hello_platunov.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A39D91-2032-494C-8A47-42000B734B98}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C156C6-57F4-42A5-A570-4A022751C92A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>First change</t>
+  </si>
+  <si>
+    <t>Second change</t>
   </si>
 </sst>
 </file>
@@ -351,9 +354,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -362,6 +367,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>